<commit_message>
Hr Process link sharing
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hr_Process\RoboticEnterpriseFramework_Hr_Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B4819A-8FD7-4119-9A8A-5BDCF57B0CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440CCF86-0433-4AE6-A5D7-144F184128E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Excel_File</t>
   </si>
   <si>
-    <t>Data\Input\Excel sheet_link sharing - Copy.xlsx</t>
-  </si>
-  <si>
     <t>Google_Meet_Url</t>
   </si>
   <si>
@@ -178,6 +175,27 @@
   </si>
   <si>
     <t>https://mail.featsystems.com/</t>
+  </si>
+  <si>
+    <t>WhatsApp_Url</t>
+  </si>
+  <si>
+    <t>https://api.whatsapp.com/send?phone=+918920781435&amp;text=Meeting%20%20link=&amp;source=&amp;data=</t>
+  </si>
+  <si>
+    <t>Data\Input\ranjit.xlsx</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ranjit.gupta@featsystems.com</t>
+  </si>
+  <si>
+    <t>Raj8052842743@</t>
+  </si>
+  <si>
+    <t>Username</t>
   </si>
 </sst>
 </file>
@@ -557,7 +575,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -627,7 +645,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="30">
@@ -643,25 +661,46 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="5" t="s">
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
         <v>50</v>
       </c>
+      <c r="B8" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>